<commit_message>
Update "Community Roles" "Community Roles.xlsx".
</commit_message>
<xml_diff>
--- a/Community Roles/Community Roles.xlsx
+++ b/Community Roles/Community Roles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssimon\Documents\GitLab\Fallen\discord-community-server\Community Roles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssimon\Documents\GitLab\fallen\discord-community-server\Community Roles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6581DA9-59A5-410A-B5AB-82E6C5002018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F4806E-05C5-48D7-8FFB-3CA0BD9972EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6C3D2279-9901-4A81-AE9E-01194CD8FEE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Role</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>DKP Master</t>
+  </si>
+  <si>
+    <t>Mod</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D96FD33-0C43-4D88-9A2D-E712441FB46F}">
-  <dimension ref="A1:BC21"/>
+  <dimension ref="A1:BC22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -922,47 +925,52 @@
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:A21">
-    <sortCondition ref="A17:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:A22">
+    <sortCondition ref="A18:A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create "Community Roles" "Community Roles.xlsx".
</commit_message>
<xml_diff>
--- a/Community Roles/Community Roles.xlsx
+++ b/Community Roles/Community Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssimon\Documents\GitLab\fallen\fallen-discord-community-server\Community Roles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F0C2D3-1081-44E2-AF97-29BCFC0B8123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44132134-F424-4F4D-B283-A0232EC445B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{6C3D2279-9901-4A81-AE9E-01194CD8FEE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{6C3D2279-9901-4A81-AE9E-01194CD8FEE7}"/>
   </bookViews>
   <sheets>
     <sheet name="050125" sheetId="17" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="050325" sheetId="19" r:id="rId3"/>
     <sheet name="050725" sheetId="20" r:id="rId4"/>
     <sheet name="050825" sheetId="21" r:id="rId5"/>
-    <sheet name="Current" sheetId="22" r:id="rId6"/>
+    <sheet name="051325" sheetId="22" r:id="rId6"/>
+    <sheet name="Current" sheetId="23" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6403" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7511" uniqueCount="86">
   <si>
     <t>Role</t>
   </si>
@@ -297,6 +298,9 @@
   <si>
     <t>Ext-AFK</t>
   </si>
+  <si>
+    <t>Paragon</t>
+  </si>
 </sst>
 </file>
 
@@ -347,7 +351,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -476,7 +499,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25337DEE-6C41-45E8-842A-008095AB529C}" name="Table1" displayName="Table1" ref="A1:BC22" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25337DEE-6C41-45E8-842A-008095AB529C}" name="Table1" displayName="Table1" ref="A1:BC22" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:BC22" xr:uid="{25337DEE-6C41-45E8-842A-008095AB529C}"/>
   <tableColumns count="55">
     <tableColumn id="1" xr3:uid="{2B2E9E74-4A9B-4E97-AC03-F5ECD4E1424A}" name="Role"/>
@@ -540,7 +563,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}" name="Table2" displayName="Table2" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}" name="Table2" displayName="Table2" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{0D48C686-A96F-412D-BC99-D5A30D8C6238}" name="Role"/>
@@ -607,7 +630,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5DB501C-9B56-45B3-87BE-C75D37C2FF87}" name="Table24" displayName="Table24" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5DB501C-9B56-45B3-87BE-C75D37C2FF87}" name="Table24" displayName="Table24" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{F802F721-228F-4D5C-82B8-A874EB147986}" name="Role"/>
@@ -674,7 +697,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03A5501D-6FB9-4029-987E-145E43D8BB6B}" name="Table245" displayName="Table245" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03A5501D-6FB9-4029-987E-145E43D8BB6B}" name="Table245" displayName="Table245" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{62C5C7CE-9663-4D8A-B0CA-33328B56533B}" name="Role"/>
@@ -741,7 +764,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ECF9E34A-2C73-4A42-810C-BBEF4B9144FB}" name="Table2456" displayName="Table2456" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ECF9E34A-2C73-4A42-810C-BBEF4B9144FB}" name="Table2456" displayName="Table2456" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:BF22" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{7EA7ADF0-B5AF-4BDA-A3A7-821826903A3F}" name="Role"/>
@@ -808,7 +831,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D17BB4-5856-4270-B44D-BF7733BCE4F0}" name="Table24567" displayName="Table24567" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D17BB4-5856-4270-B44D-BF7733BCE4F0}" name="Table24567" displayName="Table24567" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{D48B5F1A-7007-46A0-8B99-715F1B519E71}" name="Role"/>
@@ -869,6 +892,73 @@
     <tableColumn id="56" xr3:uid="{A9924A0D-55B3-4067-A41A-AF6FDCF07942}" name="Manage Events"/>
     <tableColumn id="57" xr3:uid="{BD4BFAED-D7AD-4427-BD11-B05BF44D2D74}" name="Advanced Permissions"/>
     <tableColumn id="58" xr3:uid="{B17A804F-D406-4C51-8FDD-763F8F7AB97A}" name="Administrator"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7B7D03F5-13A0-4099-833C-0531FD789F16}" name="Table245678" displayName="Table245678" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:BF22" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
+  <tableColumns count="58">
+    <tableColumn id="1" xr3:uid="{D45F072C-78E9-476A-8900-9F10ADB27876}" name="Role"/>
+    <tableColumn id="2" xr3:uid="{50823E17-2703-46EE-99D4-E07BB3AF7D22}" name="General Server Permissions"/>
+    <tableColumn id="3" xr3:uid="{F0EECECE-00D5-45BE-B440-BECE1D5D8836}" name="View Channels"/>
+    <tableColumn id="4" xr3:uid="{FDC6E70E-CF7A-4F29-9F82-6F569109C92D}" name="Manage Channels"/>
+    <tableColumn id="5" xr3:uid="{BC534A9F-C287-4D42-93F6-18EFA9A938E8}" name="Manage Roles"/>
+    <tableColumn id="6" xr3:uid="{8A98FBE8-8D5F-4C41-905B-BEC88235583E}" name="Create Expressions"/>
+    <tableColumn id="7" xr3:uid="{D5E10CA3-2A7F-4A86-806E-8FB69A094952}" name="Manage Expressions"/>
+    <tableColumn id="8" xr3:uid="{202B7B84-9614-409F-BFCE-34EFE8A4B418}" name="View Audit Log"/>
+    <tableColumn id="9" xr3:uid="{74ED500D-D68E-4A51-AA5F-598FEBB6895B}" name="View Server Insights"/>
+    <tableColumn id="10" xr3:uid="{7A12C3AE-66C9-415A-B08D-C4DD871E9ADB}" name="Manage Webhooks"/>
+    <tableColumn id="11" xr3:uid="{2B9275C0-6C24-43FF-BFBD-EEE0C31590C6}" name="Manage Server"/>
+    <tableColumn id="12" xr3:uid="{1D896D95-C3DC-40B1-837B-6BC8D21080CE}" name="Membership Permissions"/>
+    <tableColumn id="13" xr3:uid="{B7E92C63-C0BA-4A3D-8974-4A2E50113BF6}" name="Create Invite"/>
+    <tableColumn id="14" xr3:uid="{C3E8518D-7FAE-4A52-9A32-8E51D2EF1C7E}" name="Change Nickname"/>
+    <tableColumn id="15" xr3:uid="{D1801F9A-3AE1-41BD-B6F4-E2D2D0E026ED}" name="Manage Nicknames"/>
+    <tableColumn id="16" xr3:uid="{C32EF1CE-5FD5-456A-9B1F-5B8D008EF35C}" name="Kick, Approve, and Reject Members"/>
+    <tableColumn id="17" xr3:uid="{86D70326-D3C7-47F4-8581-3D9AC35F07C0}" name="Ban Members"/>
+    <tableColumn id="18" xr3:uid="{C64173EE-34C7-41B3-B570-DA2FB3720AC3}" name="Timeout Members"/>
+    <tableColumn id="19" xr3:uid="{E59D144C-3CDD-4A9C-A9A2-064C2E23B6BA}" name="Text Channel Permissions"/>
+    <tableColumn id="20" xr3:uid="{4A03C922-8B82-401C-BB02-5A92384B5D3A}" name="Send Messages"/>
+    <tableColumn id="21" xr3:uid="{E6F0FDC7-701A-4877-9CB9-46BC70FE9FA8}" name="Send Messages in Threads"/>
+    <tableColumn id="22" xr3:uid="{47B8D2F9-EEAA-4706-93B0-6F4A1285E1BA}" name="Create Public Threads"/>
+    <tableColumn id="23" xr3:uid="{6276C5B2-5D79-4C50-8857-F66E9075299D}" name="Create Private Threads"/>
+    <tableColumn id="24" xr3:uid="{AAD18AF2-05DF-4202-9295-21D51A01F75E}" name="Embed Links"/>
+    <tableColumn id="25" xr3:uid="{67E01900-632C-4DF1-887A-A25C4BEBE36F}" name="Attach Files"/>
+    <tableColumn id="26" xr3:uid="{520D74D5-2018-4CA4-BEF2-1481FF08B60B}" name="Add Reactions"/>
+    <tableColumn id="27" xr3:uid="{0698393E-902B-419E-9BFC-0A5F14B9FD12}" name="Use External Emoji"/>
+    <tableColumn id="28" xr3:uid="{CB2AAAC1-D4FB-4C30-937B-0D94A85FB88F}" name="Use External Stickers"/>
+    <tableColumn id="29" xr3:uid="{90B6429D-784A-468F-8D59-82A1AA851A1F}" name="Mention @everyone, @here, and All Roles"/>
+    <tableColumn id="30" xr3:uid="{879D857B-EF12-4DC3-AEC8-B6A5B16961A9}" name="Manage Messages"/>
+    <tableColumn id="31" xr3:uid="{79D8EC4A-4CA7-449F-9CD1-93F5C9589A48}" name="Manage Threads"/>
+    <tableColumn id="32" xr3:uid="{82DAE5C1-9B18-4758-A5BC-59FF17D61673}" name="Read Message History"/>
+    <tableColumn id="33" xr3:uid="{0953BB5A-D258-4020-9EC3-72D6746221E7}" name="Send Text-to-Speech Messages"/>
+    <tableColumn id="34" xr3:uid="{E5DB4F82-AB63-4E03-8C7A-22646A4D3F68}" name="Send Voice Messages"/>
+    <tableColumn id="35" xr3:uid="{8674098A-4A4B-4A6A-98FF-96731B5F33C1}" name="Create Polls"/>
+    <tableColumn id="36" xr3:uid="{BCF9952E-AD12-4C87-AB06-0BADF8CC261E}" name="Voice Channel Permissions"/>
+    <tableColumn id="37" xr3:uid="{1073A952-54DA-4BE1-B763-B1A1BF83C81C}" name="Connect"/>
+    <tableColumn id="38" xr3:uid="{42AC839C-BD01-47AB-9573-428DE44FB517}" name="Speak"/>
+    <tableColumn id="39" xr3:uid="{8014F761-3056-4C70-A7EF-171296B1D09A}" name="Video"/>
+    <tableColumn id="40" xr3:uid="{DB36E860-C03A-4574-8136-6B827B13E57E}" name="Use Soundboard"/>
+    <tableColumn id="41" xr3:uid="{A0A20B31-8A4C-4FBB-815E-3FA9484631F8}" name="Use External Sounds"/>
+    <tableColumn id="42" xr3:uid="{AF5E1C8C-FA1E-4890-B768-6A7406BC1BC2}" name="Use Voice Activity"/>
+    <tableColumn id="43" xr3:uid="{0270C946-423E-435A-91EF-73191573BBB9}" name="Priority Speaker"/>
+    <tableColumn id="44" xr3:uid="{9C31E792-F8E7-4D9C-92A3-0623B534B8E6}" name="Mute Members"/>
+    <tableColumn id="45" xr3:uid="{813514E1-C440-48FB-BC93-46E67FE304CF}" name="Deafen Members"/>
+    <tableColumn id="46" xr3:uid="{D710BE22-5D33-4868-9CEF-7AFDA221921B}" name="Move Members"/>
+    <tableColumn id="47" xr3:uid="{D9EB1E6B-1BFB-443E-94F1-3128E7AF0D82}" name="Set Voice Channel Status"/>
+    <tableColumn id="48" xr3:uid="{2CA3F7F3-016B-405A-BC89-B9AAA0331ED5}" name="Apps Permissions"/>
+    <tableColumn id="49" xr3:uid="{0C382486-9D6D-4E0C-B1D7-EC8D3D1E313A}" name="Use Application Commands"/>
+    <tableColumn id="50" xr3:uid="{0D8B988E-981C-4D6B-8FAB-2CAB8EE2D075}" name="Use Activities"/>
+    <tableColumn id="51" xr3:uid="{A0772412-A887-4F8F-877F-3F786C81A367}" name="Use External Apps"/>
+    <tableColumn id="52" xr3:uid="{3DDFE389-2833-42A5-BE01-8652A1044BBB}" name="Stage Channel Permissions"/>
+    <tableColumn id="53" xr3:uid="{D9E3B30F-365F-4B7C-A2E8-0531BA1CC5F8}" name="Request to Speak"/>
+    <tableColumn id="54" xr3:uid="{A2606883-B7A7-4D30-83F5-8C70AEFE0970}" name="Events Permissions"/>
+    <tableColumn id="55" xr3:uid="{1F673547-391E-4D1F-89D6-8651122FE1F3}" name="Create Events"/>
+    <tableColumn id="56" xr3:uid="{25E70B2E-C4A9-4863-841F-6E3CA16F6506}" name="Manage Events"/>
+    <tableColumn id="57" xr3:uid="{49402781-32D5-4992-9FC2-B3A47FA0D030}" name="Advanced Permissions"/>
+    <tableColumn id="58" xr3:uid="{3C6A8629-90B3-44BB-B72D-E6DE24417318}" name="Administrator"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17852,6 +17942,3304 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FDF0F7-E95C-4F56-B4F4-6D1E430B29FF}">
   <dimension ref="A1:BF21"/>
   <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:58" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W3" t="s">
+        <v>75</v>
+      </c>
+      <c r="X3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W4" t="s">
+        <v>71</v>
+      </c>
+      <c r="X4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T5" t="s">
+        <v>75</v>
+      </c>
+      <c r="U5" t="s">
+        <v>75</v>
+      </c>
+      <c r="V5" t="s">
+        <v>75</v>
+      </c>
+      <c r="W5" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R6" t="s">
+        <v>75</v>
+      </c>
+      <c r="T6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U6" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" t="s">
+        <v>75</v>
+      </c>
+      <c r="W6" t="s">
+        <v>71</v>
+      </c>
+      <c r="X6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" t="s">
+        <v>71</v>
+      </c>
+      <c r="U7" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T8" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" t="s">
+        <v>71</v>
+      </c>
+      <c r="V8" t="s">
+        <v>71</v>
+      </c>
+      <c r="W8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9" t="s">
+        <v>71</v>
+      </c>
+      <c r="V9" t="s">
+        <v>75</v>
+      </c>
+      <c r="W9" t="s">
+        <v>75</v>
+      </c>
+      <c r="X9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>75</v>
+      </c>
+      <c r="R10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" t="s">
+        <v>75</v>
+      </c>
+      <c r="U10" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" t="s">
+        <v>75</v>
+      </c>
+      <c r="W10" t="s">
+        <v>75</v>
+      </c>
+      <c r="X10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>75</v>
+      </c>
+      <c r="R11" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" t="s">
+        <v>75</v>
+      </c>
+      <c r="U11" t="s">
+        <v>75</v>
+      </c>
+      <c r="V11" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" t="s">
+        <v>75</v>
+      </c>
+      <c r="X11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R12" t="s">
+        <v>75</v>
+      </c>
+      <c r="T12" t="s">
+        <v>75</v>
+      </c>
+      <c r="U12" t="s">
+        <v>75</v>
+      </c>
+      <c r="V12" t="s">
+        <v>75</v>
+      </c>
+      <c r="W12" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" t="s">
+        <v>71</v>
+      </c>
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>75</v>
+      </c>
+      <c r="R13" t="s">
+        <v>75</v>
+      </c>
+      <c r="T13" t="s">
+        <v>75</v>
+      </c>
+      <c r="U13" t="s">
+        <v>75</v>
+      </c>
+      <c r="V13" t="s">
+        <v>75</v>
+      </c>
+      <c r="W13" t="s">
+        <v>75</v>
+      </c>
+      <c r="X13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" t="s">
+        <v>75</v>
+      </c>
+      <c r="T14" t="s">
+        <v>75</v>
+      </c>
+      <c r="U14" t="s">
+        <v>75</v>
+      </c>
+      <c r="V14" t="s">
+        <v>75</v>
+      </c>
+      <c r="W14" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>75</v>
+      </c>
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>75</v>
+      </c>
+      <c r="R15" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U15" t="s">
+        <v>75</v>
+      </c>
+      <c r="V15" t="s">
+        <v>75</v>
+      </c>
+      <c r="W15" t="s">
+        <v>75</v>
+      </c>
+      <c r="X15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" t="s">
+        <v>75</v>
+      </c>
+      <c r="P16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R16" t="s">
+        <v>75</v>
+      </c>
+      <c r="T16" t="s">
+        <v>75</v>
+      </c>
+      <c r="U16" t="s">
+        <v>75</v>
+      </c>
+      <c r="V16" t="s">
+        <v>75</v>
+      </c>
+      <c r="W16" t="s">
+        <v>75</v>
+      </c>
+      <c r="X16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N17" t="s">
+        <v>71</v>
+      </c>
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+      <c r="P17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>75</v>
+      </c>
+      <c r="R17" t="s">
+        <v>75</v>
+      </c>
+      <c r="T17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U17" t="s">
+        <v>75</v>
+      </c>
+      <c r="V17" t="s">
+        <v>75</v>
+      </c>
+      <c r="W17" t="s">
+        <v>75</v>
+      </c>
+      <c r="X17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" t="s">
+        <v>75</v>
+      </c>
+      <c r="P18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>75</v>
+      </c>
+      <c r="R18" t="s">
+        <v>75</v>
+      </c>
+      <c r="T18" t="s">
+        <v>75</v>
+      </c>
+      <c r="U18" t="s">
+        <v>75</v>
+      </c>
+      <c r="V18" t="s">
+        <v>75</v>
+      </c>
+      <c r="W18" t="s">
+        <v>75</v>
+      </c>
+      <c r="X18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" t="s">
+        <v>75</v>
+      </c>
+      <c r="T19" t="s">
+        <v>75</v>
+      </c>
+      <c r="U19" t="s">
+        <v>75</v>
+      </c>
+      <c r="V19" t="s">
+        <v>75</v>
+      </c>
+      <c r="W19" t="s">
+        <v>75</v>
+      </c>
+      <c r="X19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N20" t="s">
+        <v>71</v>
+      </c>
+      <c r="O20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>75</v>
+      </c>
+      <c r="R20" t="s">
+        <v>75</v>
+      </c>
+      <c r="T20" t="s">
+        <v>75</v>
+      </c>
+      <c r="U20" t="s">
+        <v>75</v>
+      </c>
+      <c r="V20" t="s">
+        <v>75</v>
+      </c>
+      <c r="W20" t="s">
+        <v>75</v>
+      </c>
+      <c r="X20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" t="s">
+        <v>75</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>75</v>
+      </c>
+      <c r="R21" t="s">
+        <v>75</v>
+      </c>
+      <c r="T21" t="s">
+        <v>75</v>
+      </c>
+      <c r="U21" t="s">
+        <v>75</v>
+      </c>
+      <c r="V21" t="s">
+        <v>75</v>
+      </c>
+      <c r="W21" t="s">
+        <v>75</v>
+      </c>
+      <c r="X21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35687895-CD9E-436E-9CC3-A4DCE3811747}">
+  <dimension ref="A1:BF22"/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
@@ -19467,7 +22855,7 @@
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
@@ -19619,7 +23007,7 @@
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>75</v>
@@ -19771,7 +23159,7 @@
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
@@ -19923,7 +23311,7 @@
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>75</v>
@@ -20075,7 +23463,7 @@
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>75</v>
@@ -20227,7 +23615,7 @@
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>75</v>
@@ -20379,7 +23767,7 @@
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>75</v>
@@ -20531,7 +23919,7 @@
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
         <v>75</v>
@@ -20683,7 +24071,7 @@
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
         <v>75</v>
@@ -20835,7 +24223,7 @@
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>75</v>
@@ -20987,153 +24375,305 @@
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" t="s">
+        <v>71</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>75</v>
+      </c>
+      <c r="R21" t="s">
+        <v>75</v>
+      </c>
+      <c r="T21" t="s">
+        <v>75</v>
+      </c>
+      <c r="U21" t="s">
+        <v>75</v>
+      </c>
+      <c r="V21" t="s">
+        <v>75</v>
+      </c>
+      <c r="W21" t="s">
+        <v>75</v>
+      </c>
+      <c r="X21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="C21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" t="s">
-        <v>75</v>
-      </c>
-      <c r="I21" t="s">
-        <v>75</v>
-      </c>
-      <c r="J21" t="s">
-        <v>75</v>
-      </c>
-      <c r="K21" t="s">
-        <v>75</v>
-      </c>
-      <c r="M21" t="s">
-        <v>75</v>
-      </c>
-      <c r="N21" t="s">
-        <v>75</v>
-      </c>
-      <c r="O21" t="s">
-        <v>75</v>
-      </c>
-      <c r="P21" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>75</v>
-      </c>
-      <c r="R21" t="s">
-        <v>75</v>
-      </c>
-      <c r="T21" t="s">
-        <v>75</v>
-      </c>
-      <c r="U21" t="s">
-        <v>75</v>
-      </c>
-      <c r="V21" t="s">
-        <v>75</v>
-      </c>
-      <c r="W21" t="s">
-        <v>75</v>
-      </c>
-      <c r="X21" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AS21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AT21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AW21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AY21" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA21" t="s">
-        <v>75</v>
-      </c>
-      <c r="BC21" t="s">
-        <v>75</v>
-      </c>
-      <c r="BD21" t="s">
-        <v>75</v>
-      </c>
-      <c r="BF21" t="s">
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" t="s">
+        <v>75</v>
+      </c>
+      <c r="N22" t="s">
+        <v>75</v>
+      </c>
+      <c r="O22" t="s">
+        <v>75</v>
+      </c>
+      <c r="P22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>75</v>
+      </c>
+      <c r="R22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T22" t="s">
+        <v>75</v>
+      </c>
+      <c r="U22" t="s">
+        <v>75</v>
+      </c>
+      <c r="V22" t="s">
+        <v>75</v>
+      </c>
+      <c r="W22" t="s">
+        <v>75</v>
+      </c>
+      <c r="X22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF22" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update "Community Roles" "Community Roles.xls".
</commit_message>
<xml_diff>
--- a/Community Roles/Community Roles.xlsx
+++ b/Community Roles/Community Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssimon\Documents\GitLab\fallen\fallen-discord-community-server\Community Roles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44132134-F424-4F4D-B283-A0232EC445B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA83EA25-C4E5-4109-8B1F-A0CBB4470917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{6C3D2279-9901-4A81-AE9E-01194CD8FEE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{6C3D2279-9901-4A81-AE9E-01194CD8FEE7}"/>
   </bookViews>
   <sheets>
     <sheet name="050125" sheetId="17" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="050725" sheetId="20" r:id="rId4"/>
     <sheet name="050825" sheetId="21" r:id="rId5"/>
     <sheet name="051325" sheetId="22" r:id="rId6"/>
-    <sheet name="Current" sheetId="23" r:id="rId7"/>
+    <sheet name="052425" sheetId="23" r:id="rId7"/>
+    <sheet name="Current" sheetId="24" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7511" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8569" uniqueCount="86">
   <si>
     <t>Role</t>
   </si>
@@ -351,7 +352,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -499,7 +519,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25337DEE-6C41-45E8-842A-008095AB529C}" name="Table1" displayName="Table1" ref="A1:BC22" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25337DEE-6C41-45E8-842A-008095AB529C}" name="Table1" displayName="Table1" ref="A1:BC22" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:BC22" xr:uid="{25337DEE-6C41-45E8-842A-008095AB529C}"/>
   <tableColumns count="55">
     <tableColumn id="1" xr3:uid="{2B2E9E74-4A9B-4E97-AC03-F5ECD4E1424A}" name="Role"/>
@@ -563,7 +583,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}" name="Table2" displayName="Table2" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}" name="Table2" displayName="Table2" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{0D48C686-A96F-412D-BC99-D5A30D8C6238}" name="Role"/>
@@ -630,7 +650,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5DB501C-9B56-45B3-87BE-C75D37C2FF87}" name="Table24" displayName="Table24" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5DB501C-9B56-45B3-87BE-C75D37C2FF87}" name="Table24" displayName="Table24" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{F802F721-228F-4D5C-82B8-A874EB147986}" name="Role"/>
@@ -697,7 +717,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03A5501D-6FB9-4029-987E-145E43D8BB6B}" name="Table245" displayName="Table245" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03A5501D-6FB9-4029-987E-145E43D8BB6B}" name="Table245" displayName="Table245" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{62C5C7CE-9663-4D8A-B0CA-33328B56533B}" name="Role"/>
@@ -764,7 +784,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ECF9E34A-2C73-4A42-810C-BBEF4B9144FB}" name="Table2456" displayName="Table2456" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ECF9E34A-2C73-4A42-810C-BBEF4B9144FB}" name="Table2456" displayName="Table2456" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:BF22" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{7EA7ADF0-B5AF-4BDA-A3A7-821826903A3F}" name="Role"/>
@@ -831,7 +851,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D17BB4-5856-4270-B44D-BF7733BCE4F0}" name="Table24567" displayName="Table24567" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D17BB4-5856-4270-B44D-BF7733BCE4F0}" name="Table24567" displayName="Table24567" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{D48B5F1A-7007-46A0-8B99-715F1B519E71}" name="Role"/>
@@ -898,7 +918,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7B7D03F5-13A0-4099-833C-0531FD789F16}" name="Table245678" displayName="Table245678" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7B7D03F5-13A0-4099-833C-0531FD789F16}" name="Table245678" displayName="Table245678" ref="A1:BF22" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:BF22" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
   <tableColumns count="58">
     <tableColumn id="1" xr3:uid="{D45F072C-78E9-476A-8900-9F10ADB27876}" name="Role"/>
@@ -959,6 +979,73 @@
     <tableColumn id="56" xr3:uid="{25E70B2E-C4A9-4863-841F-6E3CA16F6506}" name="Manage Events"/>
     <tableColumn id="57" xr3:uid="{49402781-32D5-4992-9FC2-B3A47FA0D030}" name="Advanced Permissions"/>
     <tableColumn id="58" xr3:uid="{3C6A8629-90B3-44BB-B72D-E6DE24417318}" name="Administrator"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7615AE6C-233F-4B77-AA21-343382C72510}" name="Table2456789" displayName="Table2456789" ref="A1:BF21" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:BF21" xr:uid="{1AE6F908-6EC8-4CC4-B1DC-44DBAD2C66F6}"/>
+  <tableColumns count="58">
+    <tableColumn id="1" xr3:uid="{6D8CBA23-362D-4997-8E42-6AB47C3B0AAE}" name="Role"/>
+    <tableColumn id="2" xr3:uid="{E5B5FF4C-C2A9-4D5E-8D2B-FCBE16200DF2}" name="General Server Permissions"/>
+    <tableColumn id="3" xr3:uid="{44708E9F-47F8-4FEF-9001-C52689D86EDE}" name="View Channels"/>
+    <tableColumn id="4" xr3:uid="{43AAFEED-9171-4AF6-8D73-FC6BFFB4E9D6}" name="Manage Channels"/>
+    <tableColumn id="5" xr3:uid="{82712D6C-3DE5-4B18-9C2B-A17AA432409F}" name="Manage Roles"/>
+    <tableColumn id="6" xr3:uid="{7624140E-3DBE-4304-B004-9CE8B8DE2D92}" name="Create Expressions"/>
+    <tableColumn id="7" xr3:uid="{A859CED5-1AF7-4E99-8985-D177C1553AF9}" name="Manage Expressions"/>
+    <tableColumn id="8" xr3:uid="{8FC4D047-D5BB-4935-8104-3561A5CF5F67}" name="View Audit Log"/>
+    <tableColumn id="9" xr3:uid="{95E59CF7-9700-4A53-A88B-DEFAB63C44CA}" name="View Server Insights"/>
+    <tableColumn id="10" xr3:uid="{44EA8A4E-6817-447F-A562-B13D95DA0135}" name="Manage Webhooks"/>
+    <tableColumn id="11" xr3:uid="{AA4FCCC2-8E52-4EE4-A60E-53BE43F74AAD}" name="Manage Server"/>
+    <tableColumn id="12" xr3:uid="{1D987E52-891C-4788-8583-14D883D9C515}" name="Membership Permissions"/>
+    <tableColumn id="13" xr3:uid="{864CF633-6B5F-47A6-8F49-89788EF3659D}" name="Create Invite"/>
+    <tableColumn id="14" xr3:uid="{9BE8E7B9-B42A-4196-9A2F-3C2E6C1F28E1}" name="Change Nickname"/>
+    <tableColumn id="15" xr3:uid="{4969AD42-5144-4130-8AC7-2EE94F84A101}" name="Manage Nicknames"/>
+    <tableColumn id="16" xr3:uid="{932B5882-0BE8-4D19-844B-F511F98AD0B7}" name="Kick, Approve, and Reject Members"/>
+    <tableColumn id="17" xr3:uid="{5AC78653-EA50-440A-A870-B7897CCE5DE7}" name="Ban Members"/>
+    <tableColumn id="18" xr3:uid="{3AC7A609-776D-4FD4-B85C-675DBEF58C8C}" name="Timeout Members"/>
+    <tableColumn id="19" xr3:uid="{9DA44528-FD60-4DE2-AE08-A940BB141123}" name="Text Channel Permissions"/>
+    <tableColumn id="20" xr3:uid="{D6ED609E-3714-456F-8F5F-92E7FDF6704B}" name="Send Messages"/>
+    <tableColumn id="21" xr3:uid="{7C3C148A-7B0D-459D-BE07-FFBA43FEC29B}" name="Send Messages in Threads"/>
+    <tableColumn id="22" xr3:uid="{6B47396D-D85F-48A9-AE92-84598F35838D}" name="Create Public Threads"/>
+    <tableColumn id="23" xr3:uid="{51B21BD9-6401-4C5B-BC28-A999CA5BA555}" name="Create Private Threads"/>
+    <tableColumn id="24" xr3:uid="{3C0A9FCA-2066-481D-8A3F-87A4B1045A18}" name="Embed Links"/>
+    <tableColumn id="25" xr3:uid="{AC120E03-9477-465B-9254-2FF67476D944}" name="Attach Files"/>
+    <tableColumn id="26" xr3:uid="{457A35FB-EA81-4762-986A-1D9998B219AC}" name="Add Reactions"/>
+    <tableColumn id="27" xr3:uid="{0F03E9B4-637B-405D-947B-7322833CD56D}" name="Use External Emoji"/>
+    <tableColumn id="28" xr3:uid="{BBA77C18-ACC6-481C-A966-DD2AA6A3C109}" name="Use External Stickers"/>
+    <tableColumn id="29" xr3:uid="{3460C3C4-159C-474D-A3F7-304E14723F7C}" name="Mention @everyone, @here, and All Roles"/>
+    <tableColumn id="30" xr3:uid="{57E5F62A-EF70-43C4-AD32-C04EEFD02B5E}" name="Manage Messages"/>
+    <tableColumn id="31" xr3:uid="{C4E259EB-3A56-4D24-92CA-C4B21A57371B}" name="Manage Threads"/>
+    <tableColumn id="32" xr3:uid="{6BE999BA-0B29-44B4-A2F7-635B07C84AD7}" name="Read Message History"/>
+    <tableColumn id="33" xr3:uid="{DCF8DCBF-BA9E-4E6A-AE20-8DAE7A0519AD}" name="Send Text-to-Speech Messages"/>
+    <tableColumn id="34" xr3:uid="{9899E985-3421-444D-ACE6-BE4C0FDCDEE6}" name="Send Voice Messages"/>
+    <tableColumn id="35" xr3:uid="{B963285B-4258-4C05-92E2-6C2BC87EA39B}" name="Create Polls"/>
+    <tableColumn id="36" xr3:uid="{AA373D0D-BB77-4D3E-98CA-CABB0F67AC7D}" name="Voice Channel Permissions"/>
+    <tableColumn id="37" xr3:uid="{788D7254-13DD-4F35-A3E2-B2E7D8383483}" name="Connect"/>
+    <tableColumn id="38" xr3:uid="{A5792D03-27E1-49D7-BB96-8E70C23EE1D5}" name="Speak"/>
+    <tableColumn id="39" xr3:uid="{A49969E7-673A-4F7C-AF79-61E5916EA6A3}" name="Video"/>
+    <tableColumn id="40" xr3:uid="{357C99F3-1B50-45FB-924B-05866BC6ABBF}" name="Use Soundboard"/>
+    <tableColumn id="41" xr3:uid="{7B8CD017-D308-4F9F-8FFB-5AC6BFC51D9C}" name="Use External Sounds"/>
+    <tableColumn id="42" xr3:uid="{AEB6674A-A193-47DF-967D-AE36B2BD706A}" name="Use Voice Activity"/>
+    <tableColumn id="43" xr3:uid="{38085B43-C6CF-46C8-8A51-743713D80860}" name="Priority Speaker"/>
+    <tableColumn id="44" xr3:uid="{35D0F0AB-0DF8-47D1-B562-6CF38864B804}" name="Mute Members"/>
+    <tableColumn id="45" xr3:uid="{6523CE14-0284-48D7-AD53-76F3CFA70400}" name="Deafen Members"/>
+    <tableColumn id="46" xr3:uid="{CC1A24C5-62D9-47AB-A943-49F1D7329A5C}" name="Move Members"/>
+    <tableColumn id="47" xr3:uid="{63ED3F50-939F-412F-A3FA-8318EB34216D}" name="Set Voice Channel Status"/>
+    <tableColumn id="48" xr3:uid="{EE0C1255-0262-4687-BCB0-EC7384D7D138}" name="Apps Permissions"/>
+    <tableColumn id="49" xr3:uid="{EB63AFD1-AB83-4C27-B991-B5F252D6B81A}" name="Use Application Commands"/>
+    <tableColumn id="50" xr3:uid="{79F35000-1F2F-417D-9585-96DAE2A836C8}" name="Use Activities"/>
+    <tableColumn id="51" xr3:uid="{A7FAAE3D-913B-4F56-98DF-3F823D8BD2BB}" name="Use External Apps"/>
+    <tableColumn id="52" xr3:uid="{7BE21AC3-A413-4466-BEC7-DCB9AA9DD458}" name="Stage Channel Permissions"/>
+    <tableColumn id="53" xr3:uid="{C48075D3-9777-426F-A032-158905AD914A}" name="Request to Speak"/>
+    <tableColumn id="54" xr3:uid="{1EC3C5C9-187A-4AC0-B79A-D1643F379BDE}" name="Events Permissions"/>
+    <tableColumn id="55" xr3:uid="{87486023-445E-48E2-9C4A-ADCC491CD016}" name="Create Events"/>
+    <tableColumn id="56" xr3:uid="{930BC840-CDA7-4DDA-8FE7-0C1FB331B4DC}" name="Manage Events"/>
+    <tableColumn id="57" xr3:uid="{5A173D14-8CAD-4F97-BD4D-8DD4CB3992A7}" name="Advanced Permissions"/>
+    <tableColumn id="58" xr3:uid="{6480192C-5D46-4A86-9BA0-318B754FB5A9}" name="Administrator"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21240,6 +21327,3456 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35687895-CD9E-436E-9CC3-A4DCE3811747}">
   <dimension ref="A1:BF22"/>
   <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:58" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W3" t="s">
+        <v>75</v>
+      </c>
+      <c r="X3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" t="s">
+        <v>71</v>
+      </c>
+      <c r="W4" t="s">
+        <v>71</v>
+      </c>
+      <c r="X4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T5" t="s">
+        <v>75</v>
+      </c>
+      <c r="U5" t="s">
+        <v>75</v>
+      </c>
+      <c r="V5" t="s">
+        <v>75</v>
+      </c>
+      <c r="W5" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R6" t="s">
+        <v>75</v>
+      </c>
+      <c r="T6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U6" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" t="s">
+        <v>75</v>
+      </c>
+      <c r="W6" t="s">
+        <v>71</v>
+      </c>
+      <c r="X6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" t="s">
+        <v>71</v>
+      </c>
+      <c r="U7" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T8" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" t="s">
+        <v>71</v>
+      </c>
+      <c r="V8" t="s">
+        <v>71</v>
+      </c>
+      <c r="W8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9" t="s">
+        <v>71</v>
+      </c>
+      <c r="V9" t="s">
+        <v>75</v>
+      </c>
+      <c r="W9" t="s">
+        <v>75</v>
+      </c>
+      <c r="X9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>75</v>
+      </c>
+      <c r="R10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" t="s">
+        <v>75</v>
+      </c>
+      <c r="U10" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" t="s">
+        <v>75</v>
+      </c>
+      <c r="W10" t="s">
+        <v>75</v>
+      </c>
+      <c r="X10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>75</v>
+      </c>
+      <c r="R11" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" t="s">
+        <v>75</v>
+      </c>
+      <c r="U11" t="s">
+        <v>75</v>
+      </c>
+      <c r="V11" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" t="s">
+        <v>75</v>
+      </c>
+      <c r="X11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R12" t="s">
+        <v>75</v>
+      </c>
+      <c r="T12" t="s">
+        <v>75</v>
+      </c>
+      <c r="U12" t="s">
+        <v>75</v>
+      </c>
+      <c r="V12" t="s">
+        <v>75</v>
+      </c>
+      <c r="W12" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" t="s">
+        <v>71</v>
+      </c>
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>75</v>
+      </c>
+      <c r="R13" t="s">
+        <v>75</v>
+      </c>
+      <c r="T13" t="s">
+        <v>75</v>
+      </c>
+      <c r="U13" t="s">
+        <v>75</v>
+      </c>
+      <c r="V13" t="s">
+        <v>75</v>
+      </c>
+      <c r="W13" t="s">
+        <v>75</v>
+      </c>
+      <c r="X13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" t="s">
+        <v>75</v>
+      </c>
+      <c r="T14" t="s">
+        <v>75</v>
+      </c>
+      <c r="U14" t="s">
+        <v>75</v>
+      </c>
+      <c r="V14" t="s">
+        <v>75</v>
+      </c>
+      <c r="W14" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>75</v>
+      </c>
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>75</v>
+      </c>
+      <c r="R15" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U15" t="s">
+        <v>75</v>
+      </c>
+      <c r="V15" t="s">
+        <v>75</v>
+      </c>
+      <c r="W15" t="s">
+        <v>75</v>
+      </c>
+      <c r="X15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" t="s">
+        <v>75</v>
+      </c>
+      <c r="P16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R16" t="s">
+        <v>75</v>
+      </c>
+      <c r="T16" t="s">
+        <v>75</v>
+      </c>
+      <c r="U16" t="s">
+        <v>75</v>
+      </c>
+      <c r="V16" t="s">
+        <v>75</v>
+      </c>
+      <c r="W16" t="s">
+        <v>75</v>
+      </c>
+      <c r="X16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N17" t="s">
+        <v>71</v>
+      </c>
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+      <c r="P17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>75</v>
+      </c>
+      <c r="R17" t="s">
+        <v>75</v>
+      </c>
+      <c r="T17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U17" t="s">
+        <v>75</v>
+      </c>
+      <c r="V17" t="s">
+        <v>75</v>
+      </c>
+      <c r="W17" t="s">
+        <v>75</v>
+      </c>
+      <c r="X17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" t="s">
+        <v>75</v>
+      </c>
+      <c r="P18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>75</v>
+      </c>
+      <c r="R18" t="s">
+        <v>75</v>
+      </c>
+      <c r="T18" t="s">
+        <v>75</v>
+      </c>
+      <c r="U18" t="s">
+        <v>75</v>
+      </c>
+      <c r="V18" t="s">
+        <v>75</v>
+      </c>
+      <c r="W18" t="s">
+        <v>75</v>
+      </c>
+      <c r="X18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" t="s">
+        <v>75</v>
+      </c>
+      <c r="T19" t="s">
+        <v>75</v>
+      </c>
+      <c r="U19" t="s">
+        <v>75</v>
+      </c>
+      <c r="V19" t="s">
+        <v>75</v>
+      </c>
+      <c r="W19" t="s">
+        <v>75</v>
+      </c>
+      <c r="X19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N20" t="s">
+        <v>71</v>
+      </c>
+      <c r="O20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>75</v>
+      </c>
+      <c r="R20" t="s">
+        <v>75</v>
+      </c>
+      <c r="T20" t="s">
+        <v>75</v>
+      </c>
+      <c r="U20" t="s">
+        <v>75</v>
+      </c>
+      <c r="V20" t="s">
+        <v>75</v>
+      </c>
+      <c r="W20" t="s">
+        <v>75</v>
+      </c>
+      <c r="X20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N21" t="s">
+        <v>71</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>75</v>
+      </c>
+      <c r="R21" t="s">
+        <v>75</v>
+      </c>
+      <c r="T21" t="s">
+        <v>75</v>
+      </c>
+      <c r="U21" t="s">
+        <v>75</v>
+      </c>
+      <c r="V21" t="s">
+        <v>75</v>
+      </c>
+      <c r="W21" t="s">
+        <v>75</v>
+      </c>
+      <c r="X21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" t="s">
+        <v>75</v>
+      </c>
+      <c r="N22" t="s">
+        <v>75</v>
+      </c>
+      <c r="O22" t="s">
+        <v>75</v>
+      </c>
+      <c r="P22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>75</v>
+      </c>
+      <c r="R22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T22" t="s">
+        <v>75</v>
+      </c>
+      <c r="U22" t="s">
+        <v>75</v>
+      </c>
+      <c r="V22" t="s">
+        <v>75</v>
+      </c>
+      <c r="W22" t="s">
+        <v>75</v>
+      </c>
+      <c r="X22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD22" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0F2CFD-99E2-4878-82F7-C9BE0FCC25D3}">
+  <dimension ref="A1:BF21"/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
@@ -23919,7 +27456,7 @@
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>75</v>
@@ -24071,7 +27608,7 @@
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>75</v>
@@ -24223,7 +27760,7 @@
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>75</v>
@@ -24375,7 +27912,7 @@
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>75</v>
@@ -24408,7 +27945,7 @@
         <v>75</v>
       </c>
       <c r="N21" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="O21" t="s">
         <v>75</v>
@@ -24522,158 +28059,6 @@
         <v>75</v>
       </c>
       <c r="BF21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" t="s">
-        <v>75</v>
-      </c>
-      <c r="J22" t="s">
-        <v>75</v>
-      </c>
-      <c r="K22" t="s">
-        <v>75</v>
-      </c>
-      <c r="M22" t="s">
-        <v>75</v>
-      </c>
-      <c r="N22" t="s">
-        <v>75</v>
-      </c>
-      <c r="O22" t="s">
-        <v>75</v>
-      </c>
-      <c r="P22" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>75</v>
-      </c>
-      <c r="R22" t="s">
-        <v>75</v>
-      </c>
-      <c r="T22" t="s">
-        <v>75</v>
-      </c>
-      <c r="U22" t="s">
-        <v>75</v>
-      </c>
-      <c r="V22" t="s">
-        <v>75</v>
-      </c>
-      <c r="W22" t="s">
-        <v>75</v>
-      </c>
-      <c r="X22" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AM22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AN22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AS22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AT22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AY22" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA22" t="s">
-        <v>75</v>
-      </c>
-      <c r="BC22" t="s">
-        <v>75</v>
-      </c>
-      <c r="BD22" t="s">
-        <v>75</v>
-      </c>
-      <c r="BF22" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>